<commit_message>
fvsOL: Manually merged changes from shinyfvsOnlineDev into this code
git-svn-id: svn+ssh://svn.code.sf.net/p/open-fvs/code/rPkgsDev@3612 90b89b48-9230-0de4-5065-812dd12741b8
</commit_message>
<xml_diff>
--- a/fvsOL/inst/extdata/databaseDescription.xlsx
+++ b/fvsOL/inst/extdata/databaseDescription.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Open-FVS\rFVS\shinyFVSOnlineDev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\FVS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7645C0CF-4F5A-48DF-AD81-A276064CC212}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68A79D3-BC7B-441E-AF3E-2D30CDC564D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="42" activeTab="45" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OutputTableDescriptions" sheetId="1" r:id="rId1"/>
@@ -71,6 +71,7 @@
     <sheet name="CmpSummary_East" sheetId="51" r:id="rId56"/>
     <sheet name="CmpSummary2" sheetId="52" r:id="rId57"/>
     <sheet name="CmpSummary2_East" sheetId="53" r:id="rId58"/>
+    <sheet name="View_DWN" sheetId="61" r:id="rId59"/>
   </sheets>
   <definedNames>
     <definedName name="OLE_LINK3" localSheetId="17">FVS_Carbon!$D$5</definedName>
@@ -87,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4981" uniqueCount="1960">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5024" uniqueCount="1968">
   <si>
     <t>Table</t>
   </si>
@@ -6048,6 +6049,30 @@
   </si>
   <si>
     <t>FVS_Regen_Ingrow</t>
+  </si>
+  <si>
+    <t>Case_ID</t>
+  </si>
+  <si>
+    <t>DWD_Total_Cover</t>
+  </si>
+  <si>
+    <t>DWD_Total_Volume</t>
+  </si>
+  <si>
+    <t>Total cover of hard and soft down wood (%)</t>
+  </si>
+  <si>
+    <t>Reported in percent cover (%). The total columns estimate the total down wood cover (3” and larger) for hard and soft wood.</t>
+  </si>
+  <si>
+    <t>Total volume of soft and hard down wood (cuft/acre)</t>
+  </si>
+  <si>
+    <t>Reported in cuft/acre. The total estimates the total down wood volume for soft and hard decay class.</t>
+  </si>
+  <si>
+    <t>is a view of the total percent cover and cubic feet per acre volume of both soft and hard downed wood, pulled from the FVS_Down_Wood_Cov and FVS_Down_Wood_Vol tables</t>
   </si>
 </sst>
 </file>
@@ -6135,7 +6160,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -6193,6 +6218,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Explanatory Text" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -6509,10 +6537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK51"/>
+  <dimension ref="A1:AMK52"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6931,6 +6959,14 @@
       </c>
       <c r="B51" s="1" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>1821</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>1967</v>
       </c>
     </row>
   </sheetData>
@@ -10585,7 +10621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B47B84-FCA3-4C5C-87A1-540887727794}">
   <dimension ref="A1:XFD53"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -29636,8 +29672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:AMK18"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29912,7 +29948,7 @@
   <dimension ref="A1:AMK20"/>
   <sheetViews>
     <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B20" sqref="B20:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35021,7 +35057,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -35326,8 +35362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
   <dimension ref="A1:AMK70"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39230,7 +39266,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3100-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -40622,6 +40658,274 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10766AA6-72AD-494C-B412-4045B85131AB}">
+  <dimension ref="A1:F33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5546875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="56.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.77734375" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>1960</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
+        <v>1437</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="s">
+        <v>798</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>799</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
+        <v>815</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>816</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="20" t="s">
+        <v>1961</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>1963</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
+        <v>833</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>834</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="20" t="s">
+        <v>851</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>852</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="20" t="s">
+        <v>1962</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>1965</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>1966</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C17" s="7"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C18" s="7"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C19" s="7"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C26" s="7"/>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMK30"/>

</xml_diff>

<commit_message>
1) The URLs in the fvsOnlineHelp.html file were updated to the new fs.usda.gov convention 2) The FVS_Carbon_Metric, FVS_SnagSum_Metric, and FVS_RD_Beetle_Metric tables were missing from the GuideLinks tab in the databaseDescription.xlsx file 3) The extension tag of the two components under Modifies > Modify Sprouting category was not being recognized. This has been resolved.
</commit_message>
<xml_diff>
--- a/fvsOL/inst/extdata/databaseDescription.xlsx
+++ b/fvsOL/inst/extdata/databaseDescription.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitFVS\ForestVegetationSimulator-Interface\fvsOLdev\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitFVS\ForestVegetationSimulator-Interface\fvsOL\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3609B0F8-B680-4A04-BF46-F829B7C4CE79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3FC6DC-1604-41A1-9C72-023F9F4EA44B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColorKey" sheetId="1" r:id="rId1"/>
@@ -123,7 +123,8 @@
     <sheet name="View_DWN_Metric" sheetId="108" r:id="rId108"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">GuideLinks!$A$1:$B$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">GuideLinks!$A$1:$B$103</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">OutputTableDescriptions!$A$1:$B$101</definedName>
     <definedName name="OLE_LINK3" localSheetId="31">FVS_Carbon!$D$5</definedName>
     <definedName name="OLE_LINK3" localSheetId="89">StdStk!$D$5</definedName>
     <definedName name="OLE_LINK3" localSheetId="91">StdStk_East!$D$5</definedName>
@@ -138,7 +139,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10030" uniqueCount="2895">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10034" uniqueCount="2895">
   <si>
     <t>Tab Color</t>
   </si>
@@ -15913,8 +15914,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+    <sheetView topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="77.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15933,788 +15934,788 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
-        <v>37</v>
+      <c r="A2" s="38" t="s">
+        <v>124</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>38</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
-        <v>12</v>
+      <c r="A3" s="34" t="s">
+        <v>126</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>2858</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="27" t="s">
-        <v>14</v>
+      <c r="A4" s="36" t="s">
+        <v>129</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>2858</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25" t="s">
-        <v>39</v>
+      <c r="A5" s="37" t="s">
+        <v>131</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>40</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27" t="s">
-        <v>41</v>
+      <c r="A6" s="35" t="s">
+        <v>128</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>2853</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="28" t="s">
-        <v>16</v>
+      <c r="A7" s="34" t="s">
+        <v>132</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>2854</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="29" t="s">
-        <v>18</v>
+      <c r="A8" s="36" t="s">
+        <v>135</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>2859</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="28" t="s">
-        <v>42</v>
+      <c r="A9" s="37" t="s">
+        <v>137</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>43</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="29" t="s">
-        <v>44</v>
+      <c r="A10" s="35" t="s">
+        <v>134</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>2852</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="25" t="s">
-        <v>45</v>
+      <c r="A11" s="34" t="s">
+        <v>138</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>46</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25" t="s">
-        <v>47</v>
+      <c r="A12" s="36" t="s">
+        <v>141</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>2855</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="27" t="s">
-        <v>48</v>
+      <c r="A13" s="37" t="s">
+        <v>143</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>2855</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="25" t="s">
-        <v>49</v>
+      <c r="A14" s="35" t="s">
+        <v>140</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>2856</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="27" t="s">
-        <v>50</v>
+      <c r="A15" s="25" t="s">
+        <v>61</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>2856</v>
+        <v>2868</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="25" t="s">
-        <v>51</v>
+      <c r="A16" s="28" t="s">
+        <v>63</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>2860</v>
+        <v>2868</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="27" t="s">
-        <v>52</v>
+      <c r="A17" s="29" t="s">
+        <v>64</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>2861</v>
+        <v>2868</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="25" t="s">
-        <v>53</v>
+      <c r="A18" s="27" t="s">
+        <v>62</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>2857</v>
+        <v>2868</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="27" t="s">
-        <v>54</v>
+      <c r="A19" s="25" t="s">
+        <v>79</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>2862</v>
+        <v>2877</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="28" t="s">
-        <v>55</v>
+      <c r="A20" s="32" t="s">
+        <v>80</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>2863</v>
+        <v>2877</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="29" t="s">
-        <v>56</v>
+      <c r="A21" s="25" t="s">
+        <v>94</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>2864</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="25" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>2865</v>
+        <v>2881</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="27" t="s">
-        <v>58</v>
+      <c r="A23" s="25" t="s">
+        <v>65</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>2866</v>
+        <v>2870</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="28" t="s">
-        <v>59</v>
+      <c r="A24" s="27" t="s">
+        <v>66</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>2867</v>
+        <v>2871</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="29" t="s">
-        <v>60</v>
+      <c r="A25" s="25" t="s">
+        <v>37</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>2867</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="25" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>2868</v>
+        <v>2885</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="27" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>2868</v>
+        <v>2885</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="28" t="s">
-        <v>63</v>
+      <c r="A28" s="25" t="s">
+        <v>45</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>2868</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="29" t="s">
-        <v>64</v>
+      <c r="A29" s="25" t="s">
+        <v>67</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>2868</v>
+        <v>2872</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="25" t="s">
-        <v>65</v>
+      <c r="A30" s="27" t="s">
+        <v>68</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>2870</v>
+        <v>2872</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="27" t="s">
-        <v>66</v>
+      <c r="A31" s="25" t="s">
+        <v>57</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>2871</v>
+        <v>2865</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="25" t="s">
-        <v>67</v>
+      <c r="A32" s="28" t="s">
+        <v>59</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>2872</v>
+        <v>2867</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="27" t="s">
-        <v>68</v>
+      <c r="A33" s="29" t="s">
+        <v>60</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>2872</v>
+        <v>2867</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="25" t="s">
+      <c r="A34" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="26" t="s">
+        <v>2866</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="26" t="s">
+        <v>2856</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="26" t="s">
+        <v>2856</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" s="26" t="s">
+        <v>2855</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" s="26" t="s">
+        <v>2855</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" s="26" t="s">
+        <v>2860</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>2861</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" s="26" t="s">
+        <v>2879</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" s="26" t="s">
+        <v>2879</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" s="26" t="s">
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" s="26" t="s">
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="B45" s="26" t="s">
+        <v>2887</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="B46" s="26" t="s">
+        <v>2887</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" s="26" t="s">
+        <v>2886</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="B48" s="26" t="s">
+        <v>2886</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B49" s="26" t="s">
+        <v>2873</v>
+      </c>
+      <c r="C49" s="33"/>
+    </row>
+    <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="B50" s="26" t="s">
+        <v>2873</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="26" t="s">
+      <c r="B51" s="26" t="s">
         <v>2869</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="27" t="s">
+    <row r="52" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="B35" s="26" t="s">
+      <c r="B52" s="26" t="s">
         <v>2869</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B36" s="26" t="s">
-        <v>2873</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="B37" s="26" t="s">
-        <v>2873</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="B38" s="26" t="s">
-        <v>2874</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="B39" s="26" t="s">
-        <v>2874</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="B40" s="26" t="s">
-        <v>2875</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="B41" s="26" t="s">
-        <v>2875</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="B42" s="26" t="s">
-        <v>2876</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="B43" s="26" t="s">
-        <v>2876</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="B44" s="26" t="s">
-        <v>2877</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="B45" s="26" t="s">
-        <v>2877</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="B46" s="26" t="s">
-        <v>2878</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="B47" s="26" t="s">
-        <v>2878</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="B48" s="26" t="s">
-        <v>2879</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="B49" s="26" t="s">
-        <v>2879</v>
-      </c>
-      <c r="C49" s="33"/>
-    </row>
-    <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="B50" s="26" t="s">
-        <v>2880</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="B51" s="26" t="s">
-        <v>2880</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="B52" s="26" t="s">
-        <v>2881</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="25" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>2882</v>
+        <v>2878</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="32" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B54" s="26" t="s">
-        <v>2882</v>
+        <v>2878</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="25" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="B55" s="26" t="s">
-        <v>2883</v>
+        <v>2874</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="32" t="s">
-        <v>91</v>
+      <c r="A56" s="25" t="s">
+        <v>77</v>
       </c>
       <c r="B56" s="26" t="s">
-        <v>2883</v>
+        <v>2876</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="25" t="s">
-        <v>92</v>
+      <c r="A57" s="32" t="s">
+        <v>78</v>
       </c>
       <c r="B57" s="26" t="s">
-        <v>2884</v>
+        <v>2876</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="27" t="s">
-        <v>93</v>
+      <c r="A58" s="28" t="s">
+        <v>75</v>
       </c>
       <c r="B58" s="26" t="s">
-        <v>2884</v>
+        <v>2875</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="25" t="s">
-        <v>94</v>
+      <c r="A59" s="31" t="s">
+        <v>76</v>
       </c>
       <c r="B59" s="26" t="s">
-        <v>95</v>
+        <v>2875</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="25" t="s">
-        <v>96</v>
+      <c r="A60" s="27" t="s">
+        <v>74</v>
       </c>
       <c r="B60" s="26" t="s">
-        <v>2885</v>
+        <v>2874</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="27" t="s">
-        <v>97</v>
+      <c r="A61" s="25" t="s">
+        <v>106</v>
       </c>
       <c r="B61" s="26" t="s">
-        <v>2885</v>
+        <v>2891</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="25" t="s">
-        <v>98</v>
+      <c r="A62" s="27" t="s">
+        <v>2890</v>
       </c>
       <c r="B62" s="26" t="s">
-        <v>2886</v>
+        <v>2891</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="32" t="s">
-        <v>99</v>
+      <c r="A63" s="25" t="s">
+        <v>104</v>
       </c>
       <c r="B63" s="26" t="s">
-        <v>2886</v>
+        <v>2889</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="25" t="s">
-        <v>100</v>
+      <c r="A64" s="27" t="s">
+        <v>105</v>
       </c>
       <c r="B64" s="26" t="s">
-        <v>2887</v>
+        <v>2889</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="27" t="s">
-        <v>101</v>
+      <c r="A65" s="25" t="s">
+        <v>102</v>
       </c>
       <c r="B65" s="26" t="s">
-        <v>2887</v>
+        <v>2888</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="25" t="s">
-        <v>102</v>
+      <c r="A66" s="27" t="s">
+        <v>103</v>
       </c>
       <c r="B66" s="26" t="s">
         <v>2888</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="27" t="s">
-        <v>103</v>
+      <c r="A67" s="25" t="s">
+        <v>115</v>
       </c>
       <c r="B67" s="26" t="s">
-        <v>2888</v>
+        <v>116</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="25" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="B68" s="26" t="s">
-        <v>2889</v>
+        <v>121</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="27" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="B69" s="26" t="s">
-        <v>2889</v>
+        <v>121</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="25" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="B70" s="26" t="s">
-        <v>2891</v>
+        <v>114</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="27" t="s">
-        <v>2890</v>
+      <c r="A71" s="25" t="s">
+        <v>110</v>
       </c>
       <c r="B71" s="26" t="s">
-        <v>2891</v>
+        <v>111</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="B72" s="22" t="s">
-        <v>2892</v>
+      <c r="A72" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="B72" s="30" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="B73" s="22" t="s">
-        <v>2892</v>
+      <c r="A73" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="B73" s="30" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="25" t="s">
-        <v>109</v>
+      <c r="A74" s="27" t="s">
+        <v>119</v>
       </c>
       <c r="B74" s="30" t="s">
-        <v>2893</v>
+        <v>118</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="25" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="B75" s="30" t="s">
-        <v>111</v>
+        <v>2883</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="27" t="s">
-        <v>112</v>
+      <c r="A76" s="32" t="s">
+        <v>91</v>
       </c>
       <c r="B76" s="30" t="s">
-        <v>111</v>
+        <v>2883</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="25" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
       <c r="B77" s="30" t="s">
-        <v>114</v>
+        <v>2882</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="25" t="s">
-        <v>115</v>
+      <c r="A78" s="32" t="s">
+        <v>89</v>
       </c>
       <c r="B78" s="30" t="s">
-        <v>116</v>
+        <v>2882</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="B79" s="30" t="s">
-        <v>118</v>
+        <v>107</v>
+      </c>
+      <c r="B79" s="22" t="s">
+        <v>2892</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="B80" s="30" t="s">
-        <v>118</v>
+        <v>108</v>
+      </c>
+      <c r="B80" s="22" t="s">
+        <v>2892</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="25" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B81" s="30" t="s">
-        <v>121</v>
+        <v>2893</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="27" t="s">
-        <v>122</v>
+      <c r="A82" s="25" t="s">
+        <v>92</v>
       </c>
       <c r="B82" s="30" t="s">
-        <v>121</v>
+        <v>2884</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="34" t="s">
-        <v>20</v>
+      <c r="A83" s="27" t="s">
+        <v>93</v>
       </c>
       <c r="B83" s="26" t="s">
-        <v>123</v>
+        <v>2884</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="35" t="s">
-        <v>22</v>
+      <c r="A84" s="25" t="s">
+        <v>12</v>
       </c>
       <c r="B84" s="26" t="s">
-        <v>123</v>
+        <v>2858</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="36" t="s">
-        <v>24</v>
+      <c r="A85" s="28" t="s">
+        <v>16</v>
       </c>
       <c r="B85" s="26" t="s">
-        <v>2894</v>
+        <v>2854</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="37" t="s">
-        <v>26</v>
+      <c r="A86" s="29" t="s">
+        <v>18</v>
       </c>
       <c r="B86" s="26" t="s">
-        <v>2894</v>
+        <v>2859</v>
       </c>
     </row>
     <row r="87" spans="1:2" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="38" t="s">
-        <v>124</v>
+      <c r="A87" s="27" t="s">
+        <v>14</v>
       </c>
       <c r="B87" s="30" t="s">
-        <v>125</v>
+        <v>2858</v>
       </c>
     </row>
     <row r="88" spans="1:2" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="34" t="s">
-        <v>126</v>
+      <c r="A88" s="25" t="s">
+        <v>39</v>
       </c>
       <c r="B88" s="30" t="s">
-        <v>127</v>
+        <v>40</v>
       </c>
     </row>
     <row r="89" spans="1:2" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="35" t="s">
-        <v>128</v>
+      <c r="A89" s="28" t="s">
+        <v>42</v>
       </c>
       <c r="B89" s="30" t="s">
-        <v>127</v>
+        <v>43</v>
       </c>
     </row>
     <row r="90" spans="1:2" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="36" t="s">
-        <v>129</v>
+      <c r="A90" s="29" t="s">
+        <v>44</v>
       </c>
       <c r="B90" s="30" t="s">
-        <v>130</v>
+        <v>2852</v>
       </c>
     </row>
     <row r="91" spans="1:2" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="37" t="s">
-        <v>131</v>
+      <c r="A91" s="27" t="s">
+        <v>41</v>
       </c>
       <c r="B91" s="30" t="s">
-        <v>130</v>
+        <v>2853</v>
       </c>
     </row>
     <row r="92" spans="1:2" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="34" t="s">
-        <v>132</v>
+      <c r="A92" s="25" t="s">
+        <v>53</v>
       </c>
       <c r="B92" s="30" t="s">
-        <v>133</v>
+        <v>2857</v>
       </c>
     </row>
     <row r="93" spans="1:2" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="35" t="s">
-        <v>134</v>
+      <c r="A93" s="28" t="s">
+        <v>55</v>
       </c>
       <c r="B93" s="30" t="s">
-        <v>133</v>
+        <v>2863</v>
       </c>
     </row>
     <row r="94" spans="1:2" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="36" t="s">
-        <v>135</v>
+      <c r="A94" s="29" t="s">
+        <v>56</v>
       </c>
       <c r="B94" s="30" t="s">
-        <v>136</v>
+        <v>2864</v>
       </c>
     </row>
     <row r="95" spans="1:2" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="37" t="s">
-        <v>137</v>
+      <c r="A95" s="27" t="s">
+        <v>54</v>
       </c>
       <c r="B95" s="30" t="s">
-        <v>136</v>
+        <v>2862</v>
       </c>
     </row>
     <row r="96" spans="1:2" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="34" t="s">
-        <v>138</v>
+        <v>20</v>
       </c>
       <c r="B96" s="30" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
     </row>
     <row r="97" spans="1:2" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="35" t="s">
-        <v>140</v>
+      <c r="A97" s="36" t="s">
+        <v>24</v>
       </c>
       <c r="B97" s="30" t="s">
-        <v>139</v>
+        <v>2894</v>
       </c>
     </row>
     <row r="98" spans="1:2" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="36" t="s">
-        <v>141</v>
+      <c r="A98" s="37" t="s">
+        <v>26</v>
       </c>
       <c r="B98" s="30" t="s">
-        <v>142</v>
+        <v>2894</v>
       </c>
     </row>
     <row r="99" spans="1:2" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="37" t="s">
-        <v>143</v>
+      <c r="A99" s="35" t="s">
+        <v>22</v>
       </c>
       <c r="B99" s="30" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
     </row>
     <row r="100" spans="1:2" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -16734,6 +16735,11 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B101" xr:uid="{00000000-0001-0000-0100-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B101">
+      <sortCondition ref="A1:A101"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
@@ -21895,10 +21901,10 @@
   <sheetPr>
     <tabColor rgb="FF0D0D0D"/>
   </sheetPr>
-  <dimension ref="A1:B101"/>
+  <dimension ref="A1:B103"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22107,249 +22113,249 @@
         <v>2844</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" s="60" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" s="96" t="s">
-        <v>2848</v>
+        <v>66</v>
+      </c>
+      <c r="B26" s="97" t="s">
+        <v>2844</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="96" t="s">
+        <v>2848</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="42" t="s">
         <v>96</v>
-      </c>
-      <c r="B27" s="96" t="s">
-        <v>2850</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="43" t="s">
-        <v>97</v>
       </c>
       <c r="B28" s="96" t="s">
         <v>2850</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" s="97" t="s">
-        <v>2845</v>
+      <c r="A29" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" s="96" t="s">
+        <v>2850</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="97" t="s">
+        <v>2845</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="42" t="s">
         <v>67</v>
-      </c>
-      <c r="B30" s="97" t="s">
-        <v>2849</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="43" t="s">
-        <v>68</v>
       </c>
       <c r="B31" s="97" t="s">
         <v>2849</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="42" t="s">
+      <c r="A32" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="97" t="s">
+        <v>2849</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="42" t="s">
         <v>57</v>
-      </c>
-      <c r="B32" s="97" t="s">
-        <v>2845</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="44" t="s">
-        <v>59</v>
       </c>
       <c r="B33" s="97" t="s">
         <v>2845</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="45" t="s">
-        <v>60</v>
+      <c r="A34" s="44" t="s">
+        <v>59</v>
       </c>
       <c r="B34" s="97" t="s">
         <v>2845</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="43" t="s">
-        <v>58</v>
+      <c r="A35" s="45" t="s">
+        <v>60</v>
       </c>
       <c r="B35" s="97" t="s">
         <v>2845</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="42" t="s">
+      <c r="A36" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" s="97" t="s">
+        <v>2845</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="42" t="s">
         <v>49</v>
-      </c>
-      <c r="B36" s="97" t="s">
-        <v>2843</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="43" t="s">
-        <v>50</v>
       </c>
       <c r="B37" s="97" t="s">
         <v>2843</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="42" t="s">
-        <v>47</v>
+      <c r="A38" s="43" t="s">
+        <v>50</v>
       </c>
       <c r="B38" s="97" t="s">
         <v>2843</v>
       </c>
     </row>
-    <row r="39" spans="1:2" s="47" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="43" t="s">
-        <v>48</v>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="42" t="s">
+        <v>47</v>
       </c>
       <c r="B39" s="97" t="s">
         <v>2843</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="42" t="s">
-        <v>51</v>
+    <row r="40" spans="1:2" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="43" t="s">
+        <v>48</v>
       </c>
       <c r="B40" s="97" t="s">
         <v>2843</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="43" t="s">
-        <v>52</v>
+      <c r="A41" s="42" t="s">
+        <v>51</v>
       </c>
       <c r="B41" s="97" t="s">
         <v>2843</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="42" t="s">
+      <c r="A42" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B42" s="97" t="s">
+        <v>2843</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="42" t="s">
         <v>83</v>
-      </c>
-      <c r="B42" s="97" t="s">
-        <v>2849</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="43" t="s">
-        <v>84</v>
       </c>
       <c r="B43" s="97" t="s">
         <v>2849</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="42" t="s">
-        <v>85</v>
+      <c r="A44" s="43" t="s">
+        <v>84</v>
       </c>
       <c r="B44" s="97" t="s">
         <v>2849</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="43" t="s">
-        <v>86</v>
+      <c r="A45" s="42" t="s">
+        <v>85</v>
       </c>
       <c r="B45" s="97" t="s">
         <v>2849</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="42" t="s">
+      <c r="A46" s="43" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" s="97" t="s">
+        <v>2849</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="42" t="s">
         <v>100</v>
-      </c>
-      <c r="B46" s="96" t="s">
-        <v>2851</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="43" t="s">
-        <v>101</v>
       </c>
       <c r="B47" s="96" t="s">
         <v>2851</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="42" t="s">
-        <v>98</v>
+      <c r="A48" s="43" t="s">
+        <v>101</v>
       </c>
       <c r="B48" s="96" t="s">
         <v>2851</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="49" t="s">
-        <v>99</v>
+      <c r="A49" s="42" t="s">
+        <v>98</v>
       </c>
       <c r="B49" s="96" t="s">
         <v>2851</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="42" t="s">
+      <c r="A50" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="B50" s="96" t="s">
+        <v>2851</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="42" t="s">
         <v>71</v>
-      </c>
-      <c r="B50" s="97" t="s">
-        <v>2849</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="43" t="s">
-        <v>72</v>
       </c>
       <c r="B51" s="97" t="s">
         <v>2849</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="42" t="s">
+      <c r="A52" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="B52" s="97" t="s">
+        <v>2849</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="42" t="s">
         <v>69</v>
-      </c>
-      <c r="B52" s="97" t="s">
-        <v>2844</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="43" t="s">
-        <v>70</v>
       </c>
       <c r="B53" s="97" t="s">
         <v>2844</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="42" t="s">
+      <c r="A54" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="B54" s="97" t="s">
+        <v>2844</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="42" t="s">
         <v>81</v>
-      </c>
-      <c r="B54" s="97" t="s">
-        <v>2849</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="48" t="s">
-        <v>82</v>
       </c>
       <c r="B55" s="97" t="s">
         <v>2849</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="42" t="s">
-        <v>73</v>
+      <c r="A56" s="48" t="s">
+        <v>82</v>
       </c>
       <c r="B56" s="97" t="s">
         <v>2849</v>
@@ -22357,54 +22363,54 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="42" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B57" s="97" t="s">
         <v>2849</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="48" t="s">
-        <v>78</v>
+      <c r="A58" s="42" t="s">
+        <v>77</v>
       </c>
       <c r="B58" s="97" t="s">
         <v>2849</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="44" t="s">
-        <v>75</v>
+      <c r="A59" s="48" t="s">
+        <v>78</v>
       </c>
       <c r="B59" s="97" t="s">
         <v>2849</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="48" t="s">
-        <v>76</v>
+      <c r="A60" s="44" t="s">
+        <v>75</v>
       </c>
       <c r="B60" s="97" t="s">
         <v>2849</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="46" t="s">
-        <v>74</v>
+      <c r="A61" s="48" t="s">
+        <v>76</v>
       </c>
       <c r="B61" s="97" t="s">
         <v>2849</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="42" t="s">
-        <v>106</v>
-      </c>
-      <c r="B62" s="96" t="s">
-        <v>2846</v>
+      <c r="A62" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="B62" s="97" t="s">
+        <v>2849</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="43" t="s">
+      <c r="A63" s="42" t="s">
         <v>106</v>
       </c>
       <c r="B63" s="96" t="s">
@@ -22412,64 +22418,64 @@
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="42" t="s">
-        <v>104</v>
+      <c r="A64" s="43" t="s">
+        <v>2890</v>
       </c>
       <c r="B64" s="96" t="s">
         <v>2846</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="43" t="s">
-        <v>105</v>
+      <c r="A65" s="42" t="s">
+        <v>104</v>
       </c>
       <c r="B65" s="96" t="s">
         <v>2846</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="42" t="s">
-        <v>102</v>
+      <c r="A66" s="43" t="s">
+        <v>105</v>
       </c>
       <c r="B66" s="96" t="s">
         <v>2846</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="43" t="s">
-        <v>103</v>
+      <c r="A67" s="42" t="s">
+        <v>102</v>
       </c>
       <c r="B67" s="96" t="s">
         <v>2846</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="42" t="s">
-        <v>115</v>
+      <c r="A68" s="43" t="s">
+        <v>103</v>
       </c>
       <c r="B68" s="96" t="s">
-        <v>2847</v>
+        <v>2846</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="42" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B69" s="96" t="s">
         <v>2847</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="43" t="s">
-        <v>122</v>
+      <c r="A70" s="42" t="s">
+        <v>120</v>
       </c>
       <c r="B70" s="96" t="s">
         <v>2847</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="42" t="s">
-        <v>113</v>
+      <c r="A71" s="43" t="s">
+        <v>122</v>
       </c>
       <c r="B71" s="96" t="s">
         <v>2847</v>
@@ -22477,55 +22483,55 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="42" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B72" s="96" t="s">
         <v>2847</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" s="43" t="s">
-        <v>112</v>
+      <c r="A73" s="42" t="s">
+        <v>110</v>
       </c>
       <c r="B73" s="96" t="s">
         <v>2847</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" s="42" t="s">
-        <v>117</v>
+      <c r="A74" s="43" t="s">
+        <v>112</v>
       </c>
       <c r="B74" s="96" t="s">
         <v>2847</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" s="43" t="s">
-        <v>119</v>
+      <c r="A75" s="42" t="s">
+        <v>117</v>
       </c>
       <c r="B75" s="96" t="s">
         <v>2847</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" s="42" t="s">
+      <c r="A76" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="B76" s="96" t="s">
+        <v>2847</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" s="42" t="s">
         <v>90</v>
-      </c>
-      <c r="B76" s="97" t="s">
-        <v>2849</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" s="48" t="s">
-        <v>91</v>
       </c>
       <c r="B77" s="97" t="s">
         <v>2849</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" s="42" t="s">
-        <v>88</v>
+      <c r="A78" s="48" t="s">
+        <v>91</v>
       </c>
       <c r="B78" s="97" t="s">
         <v>2849</v>
@@ -22533,39 +22539,39 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="42" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="B79" s="97" t="s">
-        <v>2845</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" s="43" t="s">
-        <v>108</v>
+        <v>2849</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" s="60" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="42" t="s">
+        <v>89</v>
       </c>
       <c r="B80" s="97" t="s">
-        <v>2845</v>
+        <v>2849</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="42" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B81" s="97" t="s">
         <v>2845</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" s="42" t="s">
-        <v>92</v>
+      <c r="A82" s="43" t="s">
+        <v>108</v>
       </c>
       <c r="B82" s="97" t="s">
         <v>2845</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" s="46" t="s">
-        <v>93</v>
+      <c r="A83" s="42" t="s">
+        <v>109</v>
       </c>
       <c r="B83" s="97" t="s">
         <v>2845</v>
@@ -22573,135 +22579,135 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="42" t="s">
-        <v>12</v>
+        <v>92</v>
       </c>
       <c r="B84" s="97" t="s">
         <v>2845</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" s="44" t="s">
-        <v>16</v>
+      <c r="A85" s="46" t="s">
+        <v>93</v>
       </c>
       <c r="B85" s="97" t="s">
         <v>2845</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86" s="45" t="s">
-        <v>18</v>
+      <c r="A86" s="42" t="s">
+        <v>12</v>
       </c>
       <c r="B86" s="97" t="s">
         <v>2845</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87" s="43" t="s">
-        <v>14</v>
+      <c r="A87" s="44" t="s">
+        <v>16</v>
       </c>
       <c r="B87" s="97" t="s">
         <v>2845</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A88" s="42" t="s">
-        <v>39</v>
+      <c r="A88" s="45" t="s">
+        <v>18</v>
       </c>
       <c r="B88" s="97" t="s">
         <v>2845</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A89" s="44" t="s">
-        <v>42</v>
+      <c r="A89" s="43" t="s">
+        <v>14</v>
       </c>
       <c r="B89" s="97" t="s">
         <v>2845</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A90" s="45" t="s">
-        <v>44</v>
+      <c r="A90" s="42" t="s">
+        <v>39</v>
       </c>
       <c r="B90" s="97" t="s">
         <v>2845</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A91" s="43" t="s">
-        <v>41</v>
+      <c r="A91" s="44" t="s">
+        <v>42</v>
       </c>
       <c r="B91" s="97" t="s">
         <v>2845</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A92" s="42" t="s">
-        <v>53</v>
+      <c r="A92" s="45" t="s">
+        <v>44</v>
       </c>
       <c r="B92" s="97" t="s">
         <v>2845</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A93" s="44" t="s">
-        <v>55</v>
+      <c r="A93" s="43" t="s">
+        <v>41</v>
       </c>
       <c r="B93" s="97" t="s">
         <v>2845</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A94" s="45" t="s">
-        <v>56</v>
+      <c r="A94" s="42" t="s">
+        <v>53</v>
       </c>
       <c r="B94" s="97" t="s">
         <v>2845</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A95" s="43" t="s">
-        <v>54</v>
+      <c r="A95" s="44" t="s">
+        <v>55</v>
       </c>
       <c r="B95" s="97" t="s">
         <v>2845</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A96" s="50" t="s">
+      <c r="A96" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="B96" s="97" t="s">
+        <v>2845</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="B97" s="97" t="s">
+        <v>2845</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" s="50" t="s">
         <v>20</v>
-      </c>
-      <c r="B96" s="96" t="s">
-        <v>2848</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" s="52" t="s">
-        <v>24</v>
-      </c>
-      <c r="B97" s="96" t="s">
-        <v>2848</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A98" s="53" t="s">
-        <v>26</v>
       </c>
       <c r="B98" s="96" t="s">
         <v>2848</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99" s="51" t="s">
-        <v>22</v>
+      <c r="A99" s="52" t="s">
+        <v>24</v>
       </c>
       <c r="B99" s="96" t="s">
         <v>2848</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A100" s="50" t="s">
-        <v>144</v>
+      <c r="A100" s="53" t="s">
+        <v>26</v>
       </c>
       <c r="B100" s="96" t="s">
         <v>2848</v>
@@ -22709,40 +22715,56 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="51" t="s">
-        <v>146</v>
+        <v>22</v>
       </c>
       <c r="B101" s="96" t="s">
         <v>2848</v>
       </c>
     </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" s="50" t="s">
+        <v>144</v>
+      </c>
+      <c r="B102" s="96" t="s">
+        <v>2848</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" s="51" t="s">
+        <v>146</v>
+      </c>
+      <c r="B103" s="96" t="s">
+        <v>2848</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B101" xr:uid="{00000000-0001-0000-0200-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B101">
-      <sortCondition ref="A1:A101"/>
+  <autoFilter ref="A1:B103" xr:uid="{00000000-0001-0000-0200-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B103">
+      <sortCondition ref="A1:A103"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="B26" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B27" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
     <hyperlink ref="B23" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000039000000}"/>
-    <hyperlink ref="B27" r:id="rId3" xr:uid="{00000000-0004-0000-0200-00003A000000}"/>
-    <hyperlink ref="B28" r:id="rId4" xr:uid="{00000000-0004-0000-0200-00003B000000}"/>
-    <hyperlink ref="B66" r:id="rId5" display="https://www.fs.fed.us/foresthealth/technology/pdfs/WesternRootDiseaseModelV3-0UserGuide2018.pdf" xr:uid="{00000000-0004-0000-0200-000040000000}"/>
-    <hyperlink ref="B67" r:id="rId6" display="https://www.fs.fed.us/foresthealth/technology/pdfs/WesternRootDiseaseModelV3-0UserGuide2018.pdf" xr:uid="{00000000-0004-0000-0200-000041000000}"/>
-    <hyperlink ref="B64" r:id="rId7" display="https://www.fs.fed.us/foresthealth/technology/pdfs/WesternRootDiseaseModelV3-0UserGuide2018.pdf" xr:uid="{00000000-0004-0000-0200-000042000000}"/>
-    <hyperlink ref="B65" r:id="rId8" display="https://www.fs.fed.us/foresthealth/technology/pdfs/WesternRootDiseaseModelV3-0UserGuide2018.pdf" xr:uid="{00000000-0004-0000-0200-000043000000}"/>
-    <hyperlink ref="B62" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000044000000}"/>
-    <hyperlink ref="B63" r:id="rId10" display="https://www.fs.fed.us/foresthealth/technology/pdfs/WesternRootDiseaseModelV3-0UserGuide2018.pdf" xr:uid="{00000000-0004-0000-0200-000045000000}"/>
-    <hyperlink ref="B72" r:id="rId11" display="https://www.fs.fed.us/rm/pubs_int/int_gtr279.pdf" xr:uid="{00000000-0004-0000-0200-000049000000}"/>
-    <hyperlink ref="B73" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00004A000000}"/>
-    <hyperlink ref="B71" r:id="rId13" display="https://www.fs.fed.us/rm/pubs_int/int_gtr279.pdf" xr:uid="{00000000-0004-0000-0200-00004B000000}"/>
-    <hyperlink ref="B68" r:id="rId14" display="https://www.fs.fed.us/rm/pubs_int/int_gtr279.pdf" xr:uid="{00000000-0004-0000-0200-00004C000000}"/>
-    <hyperlink ref="B74" r:id="rId15" display="https://www.fs.fed.us/rm/pubs_int/int_gtr279.pdf" xr:uid="{00000000-0004-0000-0200-00004D000000}"/>
-    <hyperlink ref="B75" r:id="rId16" display="https://www.fs.fed.us/rm/pubs_int/int_gtr279.pdf" xr:uid="{00000000-0004-0000-0200-00004E000000}"/>
-    <hyperlink ref="B69" r:id="rId17" xr:uid="{00000000-0004-0000-0200-00004F000000}"/>
-    <hyperlink ref="B70" r:id="rId18" display="https://www.fs.fed.us/rm/pubs_int/int_gtr279.pdf" xr:uid="{00000000-0004-0000-0200-000050000000}"/>
-    <hyperlink ref="B96" r:id="rId19" xr:uid="{00000000-0004-0000-0200-000051000000}"/>
-    <hyperlink ref="B99" r:id="rId20" display="https://www.fs.fed.us/.ftproot/pub/fmsc/ftp/fvs/docs/gtr/DBSUserGuide.pdf" xr:uid="{00000000-0004-0000-0200-000052000000}"/>
-    <hyperlink ref="B97" r:id="rId21" display="https://www.fs.fed.us/.ftproot/pub/fmsc/ftp/fvs/docs/gtr/DBSUserGuide.pdf" xr:uid="{00000000-0004-0000-0200-000053000000}"/>
+    <hyperlink ref="B28" r:id="rId3" xr:uid="{00000000-0004-0000-0200-00003A000000}"/>
+    <hyperlink ref="B29" r:id="rId4" xr:uid="{00000000-0004-0000-0200-00003B000000}"/>
+    <hyperlink ref="B67" r:id="rId5" display="https://www.fs.fed.us/foresthealth/technology/pdfs/WesternRootDiseaseModelV3-0UserGuide2018.pdf" xr:uid="{00000000-0004-0000-0200-000040000000}"/>
+    <hyperlink ref="B68" r:id="rId6" display="https://www.fs.fed.us/foresthealth/technology/pdfs/WesternRootDiseaseModelV3-0UserGuide2018.pdf" xr:uid="{00000000-0004-0000-0200-000041000000}"/>
+    <hyperlink ref="B65" r:id="rId7" display="https://www.fs.fed.us/foresthealth/technology/pdfs/WesternRootDiseaseModelV3-0UserGuide2018.pdf" xr:uid="{00000000-0004-0000-0200-000042000000}"/>
+    <hyperlink ref="B66" r:id="rId8" display="https://www.fs.fed.us/foresthealth/technology/pdfs/WesternRootDiseaseModelV3-0UserGuide2018.pdf" xr:uid="{00000000-0004-0000-0200-000043000000}"/>
+    <hyperlink ref="B63" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000044000000}"/>
+    <hyperlink ref="B64" r:id="rId10" display="https://www.fs.fed.us/foresthealth/technology/pdfs/WesternRootDiseaseModelV3-0UserGuide2018.pdf" xr:uid="{00000000-0004-0000-0200-000045000000}"/>
+    <hyperlink ref="B73" r:id="rId11" display="https://www.fs.fed.us/rm/pubs_int/int_gtr279.pdf" xr:uid="{00000000-0004-0000-0200-000049000000}"/>
+    <hyperlink ref="B74" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00004A000000}"/>
+    <hyperlink ref="B72" r:id="rId13" display="https://www.fs.fed.us/rm/pubs_int/int_gtr279.pdf" xr:uid="{00000000-0004-0000-0200-00004B000000}"/>
+    <hyperlink ref="B69" r:id="rId14" display="https://www.fs.fed.us/rm/pubs_int/int_gtr279.pdf" xr:uid="{00000000-0004-0000-0200-00004C000000}"/>
+    <hyperlink ref="B75" r:id="rId15" display="https://www.fs.fed.us/rm/pubs_int/int_gtr279.pdf" xr:uid="{00000000-0004-0000-0200-00004D000000}"/>
+    <hyperlink ref="B76" r:id="rId16" display="https://www.fs.fed.us/rm/pubs_int/int_gtr279.pdf" xr:uid="{00000000-0004-0000-0200-00004E000000}"/>
+    <hyperlink ref="B70" r:id="rId17" xr:uid="{00000000-0004-0000-0200-00004F000000}"/>
+    <hyperlink ref="B71" r:id="rId18" display="https://www.fs.fed.us/rm/pubs_int/int_gtr279.pdf" xr:uid="{00000000-0004-0000-0200-000050000000}"/>
+    <hyperlink ref="B98" r:id="rId19" xr:uid="{00000000-0004-0000-0200-000051000000}"/>
+    <hyperlink ref="B101" r:id="rId20" display="https://www.fs.fed.us/.ftproot/pub/fmsc/ftp/fvs/docs/gtr/DBSUserGuide.pdf" xr:uid="{00000000-0004-0000-0200-000052000000}"/>
+    <hyperlink ref="B99" r:id="rId21" display="https://www.fs.fed.us/.ftproot/pub/fmsc/ftp/fvs/docs/gtr/DBSUserGuide.pdf" xr:uid="{00000000-0004-0000-0200-000053000000}"/>
     <hyperlink ref="B5" r:id="rId22" display="https://www.fs.fed.us/.ftproot/pub/fmsc/ftp/fvs/docs/gtr/DBSUserGuide.pdf" xr:uid="{00000000-0004-0000-0200-000054000000}"/>
     <hyperlink ref="B7" r:id="rId23" display="https://www.fs.fed.us/.ftproot/pub/fmsc/ftp/fvs/docs/gtr/DBSUserGuide.pdf" xr:uid="{00000000-0004-0000-0200-000055000000}"/>
     <hyperlink ref="B10" r:id="rId24" display="https://www.fs.fed.us/.ftproot/pub/fmsc/ftp/fvs/docs/gtr/DBSUserGuide.pdf" xr:uid="{00000000-0004-0000-0200-000056000000}"/>
@@ -22752,61 +22774,62 @@
     <hyperlink ref="B14" r:id="rId28" display="https://www.fs.fed.us/.ftproot/pub/fmsc/ftp/fvs/docs/gtr/DBSUserGuide.pdf" xr:uid="{00000000-0004-0000-0200-00005A000000}"/>
     <hyperlink ref="B12" r:id="rId29" display="https://www.fs.fed.us/.ftproot/pub/fmsc/ftp/fvs/docs/gtr/DBSUserGuide.pdf" xr:uid="{00000000-0004-0000-0200-00005B000000}"/>
     <hyperlink ref="B13" r:id="rId30" display="https://www.fs.fed.us/.ftproot/pub/fmsc/ftp/fvs/docs/gtr/DBSUserGuide.pdf" xr:uid="{00000000-0004-0000-0200-00005C000000}"/>
-    <hyperlink ref="B100" r:id="rId31" display="https://www.fs.fed.us/.ftproot/pub/fmsc/ftp/fvs/docs/gtr/DBSUserGuide.pdf" xr:uid="{00000000-0004-0000-0200-00005D000000}"/>
-    <hyperlink ref="B101" r:id="rId32" display="https://www.fs.fed.us/.ftproot/pub/fmsc/ftp/fvs/docs/gtr/DBSUserGuide.pdf" xr:uid="{00000000-0004-0000-0200-00005E000000}"/>
+    <hyperlink ref="B102" r:id="rId31" display="https://www.fs.fed.us/.ftproot/pub/fmsc/ftp/fvs/docs/gtr/DBSUserGuide.pdf" xr:uid="{00000000-0004-0000-0200-00005D000000}"/>
+    <hyperlink ref="B103" r:id="rId32" display="https://www.fs.fed.us/.ftproot/pub/fmsc/ftp/fvs/docs/gtr/DBSUserGuide.pdf" xr:uid="{00000000-0004-0000-0200-00005E000000}"/>
     <hyperlink ref="B3:B11" r:id="rId33" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/EssentialFVS.pdf" xr:uid="{6CE9C5D9-2F71-47A5-BF06-D125F285F31E}"/>
-    <hyperlink ref="B18:B29" r:id="rId34" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/EssentialFVS.pdf" xr:uid="{51592308-F64A-4798-BA87-E2122C2804C7}"/>
-    <hyperlink ref="B12:B17" r:id="rId35" display="https://www.fs.usda.gov/foresthealth/technology/pdfs/DM_User_Guide_MAG-95-2_2005_nonspatial_20120627.pdf" xr:uid="{0B74CD2B-52AA-47F6-8AD6-59A69ABBF370}"/>
-    <hyperlink ref="B34:B35" r:id="rId36" display="https://www.nrs.fs.usda.gov/pubs/gtr/gtr_nrs77.pdf" xr:uid="{04F1A4D5-94B3-4437-AFD1-CF4A65768EDD}"/>
-    <hyperlink ref="B72:B74" r:id="rId37" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/EssentialFVS.pdf" xr:uid="{724622E8-AB0A-455D-A662-F4478FD6CE4A}"/>
-    <hyperlink ref="B66:B71" r:id="rId38" display="https://www.fs.usda.gov/foresthealth/technology/pdfs/WesternRootDiseaseModelV3-0UserGuide2018.pdf" xr:uid="{A45C1C7E-D416-47D7-9699-A4AC25E90D2B}"/>
-    <hyperlink ref="B2:B14" r:id="rId39" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/DBSUserGuide.pdf" xr:uid="{261A95DD-AEFB-4DFB-AD12-27CC80911E1B}"/>
-    <hyperlink ref="B15" r:id="rId40" xr:uid="{99236ADD-9300-436C-96C3-C512BE900BF9}"/>
-    <hyperlink ref="B16" r:id="rId41" xr:uid="{515E748A-8492-45EB-94A8-590F22C729CA}"/>
-    <hyperlink ref="B17" r:id="rId42" xr:uid="{58D42C0C-2BA3-456E-B574-518B4D0137C1}"/>
-    <hyperlink ref="B17:B20" r:id="rId43" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/EssentialFVS.pdf" xr:uid="{9206D5B1-629F-479E-AE22-4BCD7F14855F}"/>
-    <hyperlink ref="B21" r:id="rId44" xr:uid="{B3179AC1-3A18-43AF-BD40-D8657AC11626}"/>
-    <hyperlink ref="B22" r:id="rId45" xr:uid="{F4B95ABB-DE82-44F6-87DF-6FD6C7AE494D}"/>
-    <hyperlink ref="B21:B22" r:id="rId46" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/FFEguide.pdf" xr:uid="{CAFC0A53-672F-490A-9658-45E042FDE4D8}"/>
-    <hyperlink ref="B19" r:id="rId47" xr:uid="{7E0DD365-C578-429F-A1E9-329F35243E75}"/>
-    <hyperlink ref="B24" r:id="rId48" xr:uid="{7AA995E0-E2E4-4FB5-A35E-4089B959E0FF}"/>
-    <hyperlink ref="B25" r:id="rId49" xr:uid="{1A2F07BB-A756-4087-9A7F-D2C37880D636}"/>
-    <hyperlink ref="B3" r:id="rId50" xr:uid="{DD507D26-1866-4B46-A959-C9C474C2B06B}"/>
-    <hyperlink ref="B27:B28" r:id="rId51" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/climateFVS/ClimateFVS_UsersGuide.pdf" xr:uid="{DC8CB791-3A30-409E-8923-BDC11A9B860B}"/>
-    <hyperlink ref="B29" r:id="rId52" xr:uid="{8383C88E-47BD-44E6-96EB-693027B5DE68}"/>
-    <hyperlink ref="B30:B31" r:id="rId53" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/FFEguide.pdf" xr:uid="{D17C07AF-E9F0-46EA-A3CA-226952BDAADB}"/>
-    <hyperlink ref="B32:B35" r:id="rId54" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/EssentialFVS.pdf" xr:uid="{920435D6-665D-4AEF-AF52-6800516E8225}"/>
-    <hyperlink ref="B36" r:id="rId55" xr:uid="{5474C227-2634-480F-85A5-662E8E6D0091}"/>
-    <hyperlink ref="B36:B41" r:id="rId56" display="https://www.fs.usda.gov/foresthealth/technology/pdfs/DM_User_Guide_MAG-95-2_2005_nonspatial_20120627.pdf" xr:uid="{10B39E5E-C702-49FF-8710-97BBDED46AB3}"/>
-    <hyperlink ref="B30" r:id="rId57" xr:uid="{6F7B4C0F-EE1E-4401-B563-966067AC4DF8}"/>
-    <hyperlink ref="B42:B45" r:id="rId58" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/FFEguide.pdf" xr:uid="{5D1F4559-80C7-4675-BEDC-472837EED4CA}"/>
-    <hyperlink ref="B46:B49" r:id="rId59" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/EconUserGuide.pdf" xr:uid="{A583F457-4439-4C58-AD46-5CB86D6E99D5}"/>
-    <hyperlink ref="B42" r:id="rId60" xr:uid="{0FFE02AC-96DE-4B2A-966B-4DA4DE6EBB69}"/>
-    <hyperlink ref="B50:B51" r:id="rId61" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/FFEguide.pdf" xr:uid="{0D2FE747-AC1C-49EB-8158-FA57BB210517}"/>
-    <hyperlink ref="B52:B53" r:id="rId62" display="https://www.nrs.fs.usda.gov/pubs/gtr/gtr_nrs77.pdf" xr:uid="{D85991A4-3322-4551-A493-CB23DFF4B7B0}"/>
-    <hyperlink ref="B54:B55" r:id="rId63" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/FFEguide.pdf" xr:uid="{8CAFEC56-B459-40E8-82A9-F5A6FB1A6962}"/>
-    <hyperlink ref="B56:B57" r:id="rId64" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/FFEguide.pdf" xr:uid="{3AC6E603-58BF-4CC3-B5A6-081D533A4FFE}"/>
-    <hyperlink ref="B58:B59" r:id="rId65" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/FFEguide.pdf" xr:uid="{647569C7-260D-47CC-9148-0008679347FE}"/>
-    <hyperlink ref="B60:B61" r:id="rId66" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/FFEguide.pdf" xr:uid="{BC54E847-E9D4-4CD8-B74A-B9B9C0F0B7F0}"/>
-    <hyperlink ref="B54:B61" r:id="rId67" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/FFEguide.pdf" xr:uid="{CA3179BC-646A-4AB0-8CE3-0A1E22EBABC2}"/>
-    <hyperlink ref="B62:B67" r:id="rId68" display="https://www.fs.usda.gov/foresthealth/technology/pdfs/WesternRootDiseaseModelV3-0UserGuide2018.pdf" xr:uid="{230828C7-84A8-4D43-BD31-65033AC6CC31}"/>
-    <hyperlink ref="B68:B75" r:id="rId69" display="https://www.fs.usda.gov/rm/pubs_int/int_gtr279.pdf" xr:uid="{01104C55-42D5-4CB9-B6B4-0F8C1374BB7D}"/>
-    <hyperlink ref="B54" r:id="rId70" xr:uid="{685CAB23-0502-41D9-A9B9-4B74D7F0859D}"/>
-    <hyperlink ref="B76:B77" r:id="rId71" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/FFEguide.pdf" xr:uid="{F2C93C41-06E3-44C2-8674-ED37C386425C}"/>
-    <hyperlink ref="B78" r:id="rId72" xr:uid="{9D3ED900-B4C3-4595-83DB-BEE96C5F7E8F}"/>
-    <hyperlink ref="B76:B78" r:id="rId73" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/FFEguide.pdf" xr:uid="{80B5D81C-3F23-4B1F-AB94-8FB2D60D4A49}"/>
-    <hyperlink ref="B81:B82" r:id="rId74" display="https://www.nrs.fs.usda.gov/pubs/gtr/gtr_nrs77.pdf" xr:uid="{6092A20E-1C93-4B16-A5DC-BA33D21F49E7}"/>
-    <hyperlink ref="B79:B82" r:id="rId75" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/EssentialFVS.pdf" xr:uid="{D74048F6-2C31-4559-8786-6301519E8447}"/>
-    <hyperlink ref="B85:B86" r:id="rId76" display="https://www.nrs.fs.usda.gov/pubs/gtr/gtr_nrs77.pdf" xr:uid="{2DC19F4A-5742-45B5-BD7B-35315179DEF1}"/>
-    <hyperlink ref="B83:B86" r:id="rId77" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/EssentialFVS.pdf" xr:uid="{C5A18F86-90F0-4426-9C33-E0E474ACAAF2}"/>
-    <hyperlink ref="B89:B90" r:id="rId78" display="https://www.nrs.fs.usda.gov/pubs/gtr/gtr_nrs77.pdf" xr:uid="{C6F8C986-2E6C-4EDB-8D18-A7F0DFC14F36}"/>
-    <hyperlink ref="B87:B90" r:id="rId79" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/EssentialFVS.pdf" xr:uid="{4E57FA0B-D60A-4E6C-BB5B-5AEB658C2A22}"/>
-    <hyperlink ref="B93:B94" r:id="rId80" display="https://www.nrs.fs.usda.gov/pubs/gtr/gtr_nrs77.pdf" xr:uid="{FF3ED5FB-BF24-4947-873F-C13912D22236}"/>
-    <hyperlink ref="B91:B94" r:id="rId81" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/EssentialFVS.pdf" xr:uid="{4B8B0D61-F6A6-42D9-8C7D-C83D26C009DE}"/>
-    <hyperlink ref="B91" r:id="rId82" xr:uid="{41672F0C-92B3-416C-85B6-DD3BF44B6A75}"/>
-    <hyperlink ref="B79:B95" r:id="rId83" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/EssentialFVS.pdf" xr:uid="{FE7EEACD-BA94-4DEC-BEDF-120981E57CA1}"/>
-    <hyperlink ref="B96:B101" r:id="rId84" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/DBSUserGuide.pdf" xr:uid="{0D49BF94-3900-4073-B0CC-0EA945AA38D0}"/>
-    <hyperlink ref="B79" r:id="rId85" xr:uid="{5C0D567A-77C4-4720-899D-10CC872FA00B}"/>
+    <hyperlink ref="B12:B17" r:id="rId34" display="https://www.fs.usda.gov/foresthealth/technology/pdfs/DM_User_Guide_MAG-95-2_2005_nonspatial_20120627.pdf" xr:uid="{0B74CD2B-52AA-47F6-8AD6-59A69ABBF370}"/>
+    <hyperlink ref="B35:B36" r:id="rId35" display="https://www.nrs.fs.usda.gov/pubs/gtr/gtr_nrs77.pdf" xr:uid="{04F1A4D5-94B3-4437-AFD1-CF4A65768EDD}"/>
+    <hyperlink ref="B73:B75" r:id="rId36" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/EssentialFVS.pdf" xr:uid="{724622E8-AB0A-455D-A662-F4478FD6CE4A}"/>
+    <hyperlink ref="B67:B72" r:id="rId37" display="https://www.fs.usda.gov/foresthealth/technology/pdfs/WesternRootDiseaseModelV3-0UserGuide2018.pdf" xr:uid="{A45C1C7E-D416-47D7-9699-A4AC25E90D2B}"/>
+    <hyperlink ref="B2:B14" r:id="rId38" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/DBSUserGuide.pdf" xr:uid="{261A95DD-AEFB-4DFB-AD12-27CC80911E1B}"/>
+    <hyperlink ref="B15" r:id="rId39" xr:uid="{99236ADD-9300-436C-96C3-C512BE900BF9}"/>
+    <hyperlink ref="B16" r:id="rId40" xr:uid="{515E748A-8492-45EB-94A8-590F22C729CA}"/>
+    <hyperlink ref="B17" r:id="rId41" xr:uid="{58D42C0C-2BA3-456E-B574-518B4D0137C1}"/>
+    <hyperlink ref="B17:B20" r:id="rId42" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/EssentialFVS.pdf" xr:uid="{9206D5B1-629F-479E-AE22-4BCD7F14855F}"/>
+    <hyperlink ref="B21" r:id="rId43" xr:uid="{B3179AC1-3A18-43AF-BD40-D8657AC11626}"/>
+    <hyperlink ref="B22" r:id="rId44" xr:uid="{F4B95ABB-DE82-44F6-87DF-6FD6C7AE494D}"/>
+    <hyperlink ref="B21:B22" r:id="rId45" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/FFEguide.pdf" xr:uid="{CAFC0A53-672F-490A-9658-45E042FDE4D8}"/>
+    <hyperlink ref="B19" r:id="rId46" xr:uid="{7E0DD365-C578-429F-A1E9-329F35243E75}"/>
+    <hyperlink ref="B24" r:id="rId47" xr:uid="{7AA995E0-E2E4-4FB5-A35E-4089B959E0FF}"/>
+    <hyperlink ref="B25" r:id="rId48" xr:uid="{1A2F07BB-A756-4087-9A7F-D2C37880D636}"/>
+    <hyperlink ref="B3" r:id="rId49" xr:uid="{DD507D26-1866-4B46-A959-C9C474C2B06B}"/>
+    <hyperlink ref="B28:B29" r:id="rId50" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/climateFVS/ClimateFVS_UsersGuide.pdf" xr:uid="{DC8CB791-3A30-409E-8923-BDC11A9B860B}"/>
+    <hyperlink ref="B30" r:id="rId51" xr:uid="{8383C88E-47BD-44E6-96EB-693027B5DE68}"/>
+    <hyperlink ref="B31:B32" r:id="rId52" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/FFEguide.pdf" xr:uid="{D17C07AF-E9F0-46EA-A3CA-226952BDAADB}"/>
+    <hyperlink ref="B33:B36" r:id="rId53" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/EssentialFVS.pdf" xr:uid="{920435D6-665D-4AEF-AF52-6800516E8225}"/>
+    <hyperlink ref="B37" r:id="rId54" xr:uid="{5474C227-2634-480F-85A5-662E8E6D0091}"/>
+    <hyperlink ref="B37:B42" r:id="rId55" display="https://www.fs.usda.gov/foresthealth/technology/pdfs/DM_User_Guide_MAG-95-2_2005_nonspatial_20120627.pdf" xr:uid="{10B39E5E-C702-49FF-8710-97BBDED46AB3}"/>
+    <hyperlink ref="B31" r:id="rId56" xr:uid="{6F7B4C0F-EE1E-4401-B563-966067AC4DF8}"/>
+    <hyperlink ref="B43:B46" r:id="rId57" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/FFEguide.pdf" xr:uid="{5D1F4559-80C7-4675-BEDC-472837EED4CA}"/>
+    <hyperlink ref="B47:B50" r:id="rId58" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/EconUserGuide.pdf" xr:uid="{A583F457-4439-4C58-AD46-5CB86D6E99D5}"/>
+    <hyperlink ref="B43" r:id="rId59" xr:uid="{0FFE02AC-96DE-4B2A-966B-4DA4DE6EBB69}"/>
+    <hyperlink ref="B51:B52" r:id="rId60" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/FFEguide.pdf" xr:uid="{0D2FE747-AC1C-49EB-8158-FA57BB210517}"/>
+    <hyperlink ref="B53:B54" r:id="rId61" display="https://www.nrs.fs.usda.gov/pubs/gtr/gtr_nrs77.pdf" xr:uid="{D85991A4-3322-4551-A493-CB23DFF4B7B0}"/>
+    <hyperlink ref="B55:B56" r:id="rId62" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/FFEguide.pdf" xr:uid="{8CAFEC56-B459-40E8-82A9-F5A6FB1A6962}"/>
+    <hyperlink ref="B57:B58" r:id="rId63" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/FFEguide.pdf" xr:uid="{3AC6E603-58BF-4CC3-B5A6-081D533A4FFE}"/>
+    <hyperlink ref="B59:B60" r:id="rId64" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/FFEguide.pdf" xr:uid="{647569C7-260D-47CC-9148-0008679347FE}"/>
+    <hyperlink ref="B61:B62" r:id="rId65" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/FFEguide.pdf" xr:uid="{BC54E847-E9D4-4CD8-B74A-B9B9C0F0B7F0}"/>
+    <hyperlink ref="B55:B62" r:id="rId66" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/FFEguide.pdf" xr:uid="{CA3179BC-646A-4AB0-8CE3-0A1E22EBABC2}"/>
+    <hyperlink ref="B63:B68" r:id="rId67" display="https://www.fs.usda.gov/foresthealth/technology/pdfs/WesternRootDiseaseModelV3-0UserGuide2018.pdf" xr:uid="{230828C7-84A8-4D43-BD31-65033AC6CC31}"/>
+    <hyperlink ref="B69:B76" r:id="rId68" display="https://www.fs.usda.gov/rm/pubs_int/int_gtr279.pdf" xr:uid="{01104C55-42D5-4CB9-B6B4-0F8C1374BB7D}"/>
+    <hyperlink ref="B55" r:id="rId69" xr:uid="{685CAB23-0502-41D9-A9B9-4B74D7F0859D}"/>
+    <hyperlink ref="B77:B78" r:id="rId70" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/FFEguide.pdf" xr:uid="{F2C93C41-06E3-44C2-8674-ED37C386425C}"/>
+    <hyperlink ref="B79" r:id="rId71" xr:uid="{9D3ED900-B4C3-4595-83DB-BEE96C5F7E8F}"/>
+    <hyperlink ref="B77:B79" r:id="rId72" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/FFEguide.pdf" xr:uid="{80B5D81C-3F23-4B1F-AB94-8FB2D60D4A49}"/>
+    <hyperlink ref="B83:B84" r:id="rId73" display="https://www.nrs.fs.usda.gov/pubs/gtr/gtr_nrs77.pdf" xr:uid="{6092A20E-1C93-4B16-A5DC-BA33D21F49E7}"/>
+    <hyperlink ref="B81:B84" r:id="rId74" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/EssentialFVS.pdf" xr:uid="{D74048F6-2C31-4559-8786-6301519E8447}"/>
+    <hyperlink ref="B87:B88" r:id="rId75" display="https://www.nrs.fs.usda.gov/pubs/gtr/gtr_nrs77.pdf" xr:uid="{2DC19F4A-5742-45B5-BD7B-35315179DEF1}"/>
+    <hyperlink ref="B85:B88" r:id="rId76" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/EssentialFVS.pdf" xr:uid="{C5A18F86-90F0-4426-9C33-E0E474ACAAF2}"/>
+    <hyperlink ref="B91:B92" r:id="rId77" display="https://www.nrs.fs.usda.gov/pubs/gtr/gtr_nrs77.pdf" xr:uid="{C6F8C986-2E6C-4EDB-8D18-A7F0DFC14F36}"/>
+    <hyperlink ref="B89:B92" r:id="rId78" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/EssentialFVS.pdf" xr:uid="{4E57FA0B-D60A-4E6C-BB5B-5AEB658C2A22}"/>
+    <hyperlink ref="B95:B96" r:id="rId79" display="https://www.nrs.fs.usda.gov/pubs/gtr/gtr_nrs77.pdf" xr:uid="{FF3ED5FB-BF24-4947-873F-C13912D22236}"/>
+    <hyperlink ref="B93:B96" r:id="rId80" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/EssentialFVS.pdf" xr:uid="{4B8B0D61-F6A6-42D9-8C7D-C83D26C009DE}"/>
+    <hyperlink ref="B93" r:id="rId81" xr:uid="{41672F0C-92B3-416C-85B6-DD3BF44B6A75}"/>
+    <hyperlink ref="B81:B97" r:id="rId82" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/EssentialFVS.pdf" xr:uid="{FE7EEACD-BA94-4DEC-BEDF-120981E57CA1}"/>
+    <hyperlink ref="B98:B103" r:id="rId83" display="https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/DBSUserGuide.pdf" xr:uid="{0D49BF94-3900-4073-B0CC-0EA945AA38D0}"/>
+    <hyperlink ref="B81" r:id="rId84" xr:uid="{5C0D567A-77C4-4720-899D-10CC872FA00B}"/>
+    <hyperlink ref="B26" r:id="rId85" xr:uid="{CCFFDACD-3E7F-45A7-A1E2-D0739704B4CD}"/>
+    <hyperlink ref="B80" r:id="rId86" xr:uid="{5BE80ACC-66C8-4939-BC9C-678BE69A216A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Sn volume modifer (#55)
* Help Menu Update
Added description of Change Working Directory button to Help Screen

* Added SN merch top and stump ht to volume modifier window

* updating SN volume modifier
</commit_message>
<xml_diff>
--- a/fvsOL/inst/extdata/databaseDescription.xlsx
+++ b/fvsOL/inst/extdata/databaseDescription.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code_repos\ForestVegetationSimulator-Interface\fvsOL\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2840CB0C-E973-4A5D-8A03-C3B4E3ED2BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC54FB6-3801-439E-AAF5-C3CD67DED5AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="718" firstSheet="88" activeTab="94" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="718" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColorKey" sheetId="1" r:id="rId1"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10082" uniqueCount="2917">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10082" uniqueCount="2919">
   <si>
     <t>Tab Color</t>
   </si>
@@ -8900,6 +8900,12 @@
   </si>
   <si>
     <t>Number of stands</t>
+  </si>
+  <si>
+    <t>Trees per acre</t>
+  </si>
+  <si>
+    <t>Total Production Trees per acre</t>
   </si>
 </sst>
 </file>
@@ -13784,8 +13790,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13886,7 +13892,7 @@
         <v>193</v>
       </c>
       <c r="B7" s="52" t="s">
-        <v>268</v>
+        <v>2917</v>
       </c>
       <c r="C7" s="52" t="s">
         <v>174</v>
@@ -13900,7 +13906,7 @@
         <v>324</v>
       </c>
       <c r="B8" s="52" t="s">
-        <v>340</v>
+        <v>2918</v>
       </c>
       <c r="C8" s="52" t="s">
         <v>174</v>
@@ -46707,7 +46713,7 @@
   </sheetPr>
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Cc adj lang update (#70)
* Fixes bug where blank line in keyword list inserted in GAK caused crash

* Added SpeciesFVSnum description to CmpCalibStats / CalibStats help menus

* Address CCAdj language update
Corrects minor 508 Accessibility Issues
</commit_message>
<xml_diff>
--- a/fvsOL/inst/extdata/databaseDescription.xlsx
+++ b/fvsOL/inst/extdata/databaseDescription.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code_repos\ForestVegetationSimulator-Interface\fvsOL\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\stable_repos\ForestVegetationSimulator-Interface\fvsOL\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC54FB6-3801-439E-AAF5-C3CD67DED5AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A4EA10-02FE-47E1-B733-B4C16DD66541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="718" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5835" yWindow="330" windowWidth="25500" windowHeight="15600" tabRatio="718" firstSheet="86" activeTab="94" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColorKey" sheetId="1" r:id="rId1"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10082" uniqueCount="2919">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10090" uniqueCount="2922">
   <si>
     <t>Tab Color</t>
   </si>
@@ -8906,6 +8906,15 @@
   </si>
   <si>
     <t>Total Production Trees per acre</t>
+  </si>
+  <si>
+    <t>SpeciesFVSnum</t>
+  </si>
+  <si>
+    <t>FVS Species Number</t>
+  </si>
+  <si>
+    <t>The variant specific sequential FVS species number</t>
   </si>
 </sst>
 </file>
@@ -9384,9 +9393,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -9424,7 +9433,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -9530,7 +9539,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -9672,7 +9681,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -13790,7 +13799,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -16271,7 +16280,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ102"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -34713,10 +34722,10 @@
   <sheetPr>
     <tabColor rgb="FF203864"/>
   </sheetPr>
-  <dimension ref="A1:AMJ12"/>
+  <dimension ref="A1:AMJ13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34785,114 +34794,128 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
-        <v>529</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>530</v>
-      </c>
-      <c r="C5" s="22" t="s">
+      <c r="A5" s="36" t="s">
+        <v>2919</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>2920</v>
+      </c>
+      <c r="C5" s="36" t="s">
         <v>155</v>
       </c>
-      <c r="D5" s="22" t="s">
-        <v>531</v>
+      <c r="D5" s="36" t="s">
+        <v>2921</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="C6" s="22" t="s">
         <v>155</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="C7" s="22" t="s">
         <v>155</v>
       </c>
       <c r="D7" s="22" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>535</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>536</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="D8" s="22" t="s">
         <v>537</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
-        <v>1662</v>
-      </c>
-      <c r="B8" s="36" t="s">
-        <v>1663</v>
-      </c>
-      <c r="C8" s="36" t="s">
-        <v>189</v>
-      </c>
-      <c r="D8" s="36" t="s">
-        <v>1664</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
-        <v>1665</v>
+        <v>1662</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>1666</v>
+        <v>1663</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>1667</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36" t="s">
-        <v>1668</v>
+        <v>1665</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>1669</v>
+        <v>1666</v>
       </c>
       <c r="C10" s="36" t="s">
         <v>174</v>
       </c>
       <c r="D10" s="36" t="s">
-        <v>1670</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
-        <v>1671</v>
+        <v>1668</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>1672</v>
+        <v>1669</v>
       </c>
       <c r="C11" s="36" t="s">
         <v>174</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>1673</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>1672</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>1673</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="36" t="s">
         <v>1674</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B13" s="36" t="s">
         <v>1675</v>
       </c>
-      <c r="C12" s="36" t="s">
-        <v>174</v>
-      </c>
-      <c r="D12" s="36" t="s">
+      <c r="C13" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="D13" s="36" t="s">
         <v>2907</v>
       </c>
     </row>
@@ -46711,10 +46734,10 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46769,118 +46792,132 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1659</v>
-      </c>
-      <c r="B4" s="55" t="s">
-        <v>1660</v>
+        <v>2919</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2920</v>
       </c>
       <c r="C4" s="36" t="s">
         <v>155</v>
       </c>
       <c r="D4" s="55" t="s">
-        <v>1661</v>
+        <v>2921</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2914</v>
+        <v>1659</v>
       </c>
       <c r="B5" s="55" t="s">
-        <v>2916</v>
+        <v>1660</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>189</v>
+        <v>155</v>
       </c>
       <c r="D5" s="55" t="s">
-        <v>2915</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2895</v>
-      </c>
-      <c r="B6" t="s">
-        <v>2909</v>
-      </c>
-      <c r="C6" t="s">
-        <v>174</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2901</v>
+        <v>2914</v>
+      </c>
+      <c r="B6" s="55" t="s">
+        <v>2916</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="D6" s="55" t="s">
+        <v>2915</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="B7" t="s">
-        <v>2911</v>
+        <v>2909</v>
       </c>
       <c r="C7" t="s">
         <v>174</v>
       </c>
       <c r="D7" t="s">
-        <v>2902</v>
+        <v>2901</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="B8" t="s">
-        <v>2910</v>
+        <v>2911</v>
       </c>
       <c r="C8" t="s">
         <v>174</v>
       </c>
       <c r="D8" t="s">
-        <v>2903</v>
+        <v>2902</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="B9" t="s">
-        <v>2912</v>
+        <v>2910</v>
       </c>
       <c r="C9" t="s">
         <v>174</v>
       </c>
       <c r="D9" t="s">
-        <v>2904</v>
+        <v>2903</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2899</v>
+        <v>2898</v>
       </c>
       <c r="B10" t="s">
-        <v>2908</v>
-      </c>
-      <c r="C10" s="36" t="s">
-        <v>189</v>
+        <v>2912</v>
+      </c>
+      <c r="C10" t="s">
+        <v>174</v>
       </c>
       <c r="D10" t="s">
-        <v>2905</v>
+        <v>2904</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>2899</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2908</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2905</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>2900</v>
       </c>
-      <c r="B11" s="55" t="s">
+      <c r="B12" s="55" t="s">
         <v>1675</v>
       </c>
-      <c r="C11" t="s">
-        <v>174</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C12" t="s">
+        <v>174</v>
+      </c>
+      <c r="D12" t="s">
         <v>2906</v>
       </c>
     </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F23" s="36"/>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>